<commit_message>
Última atualização de cronograma
</commit_message>
<xml_diff>
--- a/02-Projeto/01-ResolveAi/04-Cronograma.xlsx
+++ b/02-Projeto/01-ResolveAi/04-Cronograma.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
   <si>
     <t>Cronograma Resolve Aí</t>
   </si>
@@ -171,10 +171,10 @@
     <t>Todas as atividades previstas até o momento foram concluídas.</t>
   </si>
   <si>
-    <t>Em andamento</t>
-  </si>
-  <si>
-    <t>Documento de requisitos enviado ao cliente para aprovação.</t>
+    <t>Aprovação adquirida.</t>
+  </si>
+  <si>
+    <t>Todos confirmaram comprometimento e aprovaram os requisitos.</t>
   </si>
 </sst>
 </file>
@@ -758,7 +758,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1368,10 +1368,10 @@
         <v>12</v>
       </c>
       <c r="H22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
@@ -1391,13 +1391,17 @@
         <v>18</v>
       </c>
       <c r="F23" s="9">
-        <v>43059</v>
+        <v>43062</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="10"/>
+      <c r="H23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
@@ -1421,8 +1425,12 @@
       <c r="G24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="8"/>
-      <c r="I24" s="10"/>
+      <c r="H24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>